<commit_message>
add vaadin components to spreadsheet table and created some ticket to improve API and reduce frustration for developers
</commit_message>
<xml_diff>
--- a/src/main/resources/simple-invoice.xlsx
+++ b/src/main/resources/simple-invoice.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sebastian/Documents/Vaadin/labaratory/hackthon-24/my-app/src/main/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sebastian/Documents/Vaadin/labaratory/hackthon-24/hackathon-24-0/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DE7D383-DA88-0944-9D48-8A8859FFA5C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01E5E8A9-1B4B-2D4C-8BB8-72296722037D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="880" windowWidth="41120" windowHeight="24520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -162,7 +162,7 @@
       <name val="Open Sans"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -173,6 +173,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFD8D8D8"/>
         <bgColor rgb="FFD8D8D8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -237,10 +243,10 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="6" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>

</xml_diff>